<commit_message>
Developed code for overloaded function Transpose.
</commit_message>
<xml_diff>
--- a/Time_sheet.xlsx
+++ b/Time_sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>DATE</t>
   </si>
@@ -95,6 +95,26 @@
     <t>OSR_matrix.h - Reworked overloaded set_element(), overloaded get_element().
 OSR_matrix.cpp - Put in all functions from OSR_matrix.h. Added overloaded operator= and overloaded operator+=.
 Odyssey_matrix.cpp - test of overloaded operator= and overloaded operator+=.</t>
+  </si>
+  <si>
+    <t>OSR_matrix.h - Added overloaded operator* (scalar).
+OSR_matrix.cpp - Added overloaded operator* (scalar).
+Odessey_matrix.cpp - Test for  overloaded operator* (scalar).</t>
+  </si>
+  <si>
+    <t>Overloaded operator* (matrix).</t>
+  </si>
+  <si>
+    <t>OSR_matrix.h - Added overloaded operator* (matrix).
+OSR_matrix.cpp - Added overloaded operator* (matrix).</t>
+  </si>
+  <si>
+    <t>Overloaded Function Transpose.</t>
+  </si>
+  <si>
+    <t>OSR_matrix.h - Overloaded Function Transpose.
+OSR_matrix.cpp - Overloaded Function Transpose.
+Odessey_matrix.cpp - Test for  Overloaded Function Transpose.</t>
   </si>
 </sst>
 </file>
@@ -128,7 +148,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -437,24 +457,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -467,7 +505,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -475,28 +512,16 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -516,12 +541,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -564,14 +583,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -874,36 +933,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="20" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="33" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="36" customWidth="1"/>
+    <col min="3" max="3" width="8" style="36" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="37" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="20" customWidth="1"/>
     <col min="6" max="6" width="109.85546875" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="49"/>
+    <col min="10" max="10" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -911,100 +972,100 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="50">
+      <c r="A2" s="46">
         <v>43621</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="22">
         <v>0.39583333333333331</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="22">
         <v>0.52083333333333337</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="11">
         <f t="shared" ref="D2:D15" si="0">C2-B2</f>
         <v>0.12500000000000006</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51"/>
-      <c r="B3" s="6">
+      <c r="A3" s="48"/>
+      <c r="B3" s="38">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="38">
         <v>0.79166666666666663</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="12">
         <f t="shared" si="0"/>
         <v>0.20833333333333326</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8">
+      <c r="A4" s="4">
         <v>43622</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="5">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="5">
         <v>0.64583333333333337</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="10">
         <f t="shared" si="0"/>
         <v>0.10416666666666674</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="50">
+      <c r="A5" s="46">
         <v>43623</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="22">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="22">
         <v>0.5</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="11">
         <f t="shared" si="0"/>
         <v>8.3333333333333315E-2</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="51"/>
-      <c r="B6" s="2">
+      <c r="A6" s="48"/>
+      <c r="B6" s="24">
         <v>0.625</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="24">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="12">
         <f t="shared" si="0"/>
         <v>0.20833333333333337</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -1012,209 +1073,316 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="50">
+      <c r="A7" s="46">
         <v>43624</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="39">
         <v>0.52083333333333337</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="39">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="40">
         <f t="shared" si="0"/>
         <v>0.14583333333333326</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="51"/>
-      <c r="B8" s="24">
+      <c r="A8" s="48"/>
+      <c r="B8" s="41">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="38">
         <v>0.75</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="12">
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="51.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="50">
+      <c r="A9" s="46">
         <v>43625</v>
       </c>
-      <c r="B9" s="36">
+      <c r="B9" s="21">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="22">
         <v>0.61458333333333337</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="11">
         <f t="shared" si="0"/>
         <v>7.2916666666666741E-2</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="F9" s="23" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="51"/>
-      <c r="B10" s="39">
+      <c r="A10" s="48"/>
+      <c r="B10" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C10" s="39">
+      <c r="C10" s="24">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="25">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="41" t="s">
+      <c r="F10" s="26" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="50">
+      <c r="A11" s="46">
         <v>43626</v>
       </c>
-      <c r="B11" s="36">
+      <c r="B11" s="21">
         <v>0.5</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="22">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="11">
         <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="42" t="s">
+      <c r="F11" s="27" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="52"/>
-      <c r="B12" s="45">
+      <c r="A12" s="47"/>
+      <c r="B12" s="30">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C12" s="46">
+      <c r="C12" s="31">
         <v>0.6875</v>
       </c>
-      <c r="D12" s="47">
+      <c r="D12" s="32">
         <f t="shared" si="0"/>
         <v>0.14583333333333337</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="44" t="s">
+      <c r="F12" s="29" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="51"/>
-      <c r="B13" s="39">
+      <c r="A13" s="48"/>
+      <c r="B13" s="24">
         <v>0.75</v>
       </c>
-      <c r="C13" s="39">
+      <c r="C13" s="24">
         <v>0.80208333333333337</v>
       </c>
-      <c r="D13" s="40">
+      <c r="D13" s="25">
         <f t="shared" si="0"/>
         <v>5.208333333333337E-2</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="41" t="s">
+      <c r="F13" s="26" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8">
+      <c r="A14" s="4">
         <v>43627</v>
       </c>
-      <c r="B14" s="48">
+      <c r="B14" s="33">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="5">
         <v>0.79166666666666663</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="10">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="49" t="s">
+      <c r="F14" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
+      <c r="A15" s="4">
         <v>43628</v>
       </c>
-      <c r="B15" s="48">
+      <c r="B15" s="33">
         <v>0.375</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="5">
         <v>0.70833333333333337</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="10">
         <f t="shared" si="0"/>
         <v>0.33333333333333337</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="49" t="s">
+      <c r="F15" s="34" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8">
+      <c r="A16" s="4">
         <v>43629</v>
       </c>
-      <c r="B16" s="48">
+      <c r="B16" s="33">
         <v>0.375</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="5">
         <v>0.75</v>
       </c>
-      <c r="D16" s="17">
-        <f t="shared" ref="D16" si="1">C16-B16</f>
+      <c r="D16" s="10">
+        <f t="shared" ref="D16:D21" si="1">C16-B16</f>
         <v>0.375</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="49" t="s">
+      <c r="F16" s="34" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="46">
+        <v>43630</v>
+      </c>
+      <c r="B17" s="21">
+        <v>0.4375</v>
+      </c>
+      <c r="C17" s="22">
+        <v>0.5625</v>
+      </c>
+      <c r="D17" s="11">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="47"/>
+      <c r="B18" s="42">
+        <v>0.625</v>
+      </c>
+      <c r="C18" s="42">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D18" s="43">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666663</v>
+      </c>
+      <c r="E18" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="48"/>
+      <c r="B19" s="24">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C19" s="24">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D19" s="25">
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="46">
+        <v>43631</v>
+      </c>
+      <c r="B20" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="C20" s="22">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D20" s="11">
+        <f t="shared" si="1"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="51" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="48"/>
+      <c r="B21" s="24">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C21" s="24">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D21" s="25">
+        <f t="shared" si="1"/>
+        <v>0.3125</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="35"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="35"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A17:A19"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
@@ -1222,18 +1390,475 @@
     <mergeCell ref="A11:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="22">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="B1" s="49">
+        <v>930</v>
+      </c>
+      <c r="C1" s="49">
+        <v>1230</v>
+      </c>
+      <c r="D1" s="49">
+        <f>C1-B1</f>
+        <v>300</v>
+      </c>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="38">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="B2" s="49">
+        <v>1400</v>
+      </c>
+      <c r="C2" s="49">
+        <v>1900</v>
+      </c>
+      <c r="D2" s="49">
+        <f>C2-B2</f>
+        <v>500</v>
+      </c>
+      <c r="E2" s="12"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B3" s="49">
+        <v>1300</v>
+      </c>
+      <c r="C3" s="49">
+        <v>1530</v>
+      </c>
+      <c r="D3" s="49">
+        <f>C3-B3</f>
+        <v>230</v>
+      </c>
+      <c r="E3" s="10"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="22">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B4" s="49">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="49">
+        <v>1200</v>
+      </c>
+      <c r="D4" s="49">
+        <f>C4-B4</f>
+        <v>200</v>
+      </c>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="24">
+        <v>0.625</v>
+      </c>
+      <c r="B5" s="49">
+        <v>1500</v>
+      </c>
+      <c r="C5" s="49">
+        <v>2000</v>
+      </c>
+      <c r="D5" s="49">
+        <f>C5-B5</f>
+        <v>500</v>
+      </c>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="39">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="B6" s="49">
+        <v>1230</v>
+      </c>
+      <c r="C6" s="49">
+        <v>1600</v>
+      </c>
+      <c r="D6" s="49">
+        <f>C6-B6</f>
+        <v>370</v>
+      </c>
+      <c r="E6" s="40"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="41">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="B7" s="49">
+        <v>1600</v>
+      </c>
+      <c r="C7" s="49">
+        <v>1800</v>
+      </c>
+      <c r="D7" s="49">
+        <f>C7-B7</f>
+        <v>200</v>
+      </c>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B8" s="49">
+        <v>1300</v>
+      </c>
+      <c r="C8" s="49">
+        <v>1445</v>
+      </c>
+      <c r="D8" s="49">
+        <f>C8-B8</f>
+        <v>145</v>
+      </c>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="24">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="B9" s="49">
+        <v>1700</v>
+      </c>
+      <c r="C9" s="49">
+        <v>2000</v>
+      </c>
+      <c r="D9" s="49">
+        <f>C9-B9</f>
+        <v>300</v>
+      </c>
+      <c r="E9" s="25"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="B10" s="49">
+        <v>1200</v>
+      </c>
+      <c r="C10" s="49">
+        <v>1300</v>
+      </c>
+      <c r="D10" s="49">
+        <f>C10-B10</f>
+        <v>100</v>
+      </c>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="30">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B11" s="49">
+        <v>1300</v>
+      </c>
+      <c r="C11" s="49">
+        <v>1630</v>
+      </c>
+      <c r="D11" s="49">
+        <f>C11-B11</f>
+        <v>330</v>
+      </c>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="B12" s="49">
+        <v>1800</v>
+      </c>
+      <c r="C12" s="49">
+        <v>1915</v>
+      </c>
+      <c r="D12" s="49">
+        <f>C12-B12</f>
+        <v>115</v>
+      </c>
+      <c r="E12" s="25"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="33">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B13" s="49">
+        <v>1300</v>
+      </c>
+      <c r="C13" s="49">
+        <v>1900</v>
+      </c>
+      <c r="D13" s="49">
+        <f>C13-B13</f>
+        <v>600</v>
+      </c>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="33">
+        <v>0.375</v>
+      </c>
+      <c r="B14" s="49">
+        <v>900</v>
+      </c>
+      <c r="C14" s="49">
+        <v>1700</v>
+      </c>
+      <c r="D14" s="49">
+        <f>C14-B14</f>
+        <v>800</v>
+      </c>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="33">
+        <v>0.375</v>
+      </c>
+      <c r="B15" s="49">
+        <v>900</v>
+      </c>
+      <c r="C15" s="49">
+        <v>1800</v>
+      </c>
+      <c r="D15" s="49">
+        <f>C15-B15</f>
+        <v>900</v>
+      </c>
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="21">
+        <v>0.4375</v>
+      </c>
+      <c r="B16" s="49">
+        <v>1030</v>
+      </c>
+      <c r="C16" s="49">
+        <v>1330</v>
+      </c>
+      <c r="D16" s="49">
+        <f>C16-B16</f>
+        <v>300</v>
+      </c>
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="42">
+        <v>0.625</v>
+      </c>
+      <c r="B17" s="49">
+        <v>1500</v>
+      </c>
+      <c r="C17" s="49">
+        <v>1900</v>
+      </c>
+      <c r="D17" s="49">
+        <f>C17-B17</f>
+        <v>400</v>
+      </c>
+      <c r="E17" s="43"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="24">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="B18" s="49">
+        <v>1900</v>
+      </c>
+      <c r="C18" s="49">
+        <v>2030</v>
+      </c>
+      <c r="D18" s="49">
+        <f>C18-B18</f>
+        <v>130</v>
+      </c>
+      <c r="E18" s="25"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="50"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="50"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="22">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="B21" s="49">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="38">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="B22" s="49">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="B23" s="49">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="B24" s="49">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="24">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="B25" s="49">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="39">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="B26" s="49">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="38">
+        <v>0.75</v>
+      </c>
+      <c r="B27" s="49">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="22">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="B28" s="49">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="24">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="B29" s="49">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="22">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B30" s="49">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="31">
+        <v>0.6875</v>
+      </c>
+      <c r="B31" s="49">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="24">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="B32" s="49">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="B33" s="49">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="5">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="B34" s="49">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="B35" s="49">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="22">
+        <v>0.5625</v>
+      </c>
+      <c r="B36" s="49">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="42">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="B37" s="49">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="24">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="B38" s="49">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="49"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="49"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="49"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="49"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>